<commit_message>
Problem Analyse und Ursache-Wirkung Diagramm für Idee 1
</commit_message>
<xml_diff>
--- a/Projektplan.xlsx
+++ b/Projektplan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\6. Semester\EIS\EISSS19SchoenbergerTissen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCF26ED-9983-428D-A73E-608EB44188D7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122D3B41-39CA-438B-AF5F-5E779A8102AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{B7844FFE-8D7C-4A1B-B32C-F7C7EEEB357D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Meilenstein</t>
   </si>
@@ -69,10 +69,22 @@
     <t>Malte Schönberger</t>
   </si>
   <si>
-    <t>Beratungstermin buchen</t>
-  </si>
-  <si>
     <t>EISSS19 Projektplan von Schönberger &amp; Tissen</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>Lebensmittelverschwendung</t>
+  </si>
+  <si>
+    <t>Videospielsammlung</t>
+  </si>
+  <si>
+    <t>Domänenmodell</t>
+  </si>
+  <si>
+    <t>Ursache-Wirkung Diagramm</t>
   </si>
 </sst>
 </file>
@@ -119,7 +131,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -159,6 +171,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,14 +308,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -300,6 +322,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -614,37 +638,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF5B1E5-DD07-4D84-8DF8-E9B8F5348EC4}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.33203125" customWidth="1"/>
-    <col min="2" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="6" width="20" customWidth="1"/>
+    <col min="1" max="2" width="33.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5" x14ac:dyDescent="0.85">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -654,67 +679,104 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="19"/>
+      <c r="C9" s="13">
         <v>1</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="11">
+      <c r="E9" s="10">
         <v>0.125</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="5">
         <v>0.125</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="9"/>
+      <c r="B11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F12" s="5">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="19"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="F13" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="11">
+      <c r="B14" s="19"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="10">
         <v>0.20833333333333334</v>
       </c>
-      <c r="E10" s="6">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="10"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="5"/>
+      <c r="F14" s="5">
+        <v>0.16666666666666666</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>